<commit_message>
Cập nhật bản chính thức cho tất cả tài liệu
</commit_message>
<xml_diff>
--- a/Document/Release-Plan.xlsx
+++ b/Document/Release-Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hoc_Tap\Nam 4 KHTN\HKI\QLDA\HoatDong\Noplan2_Nhom1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="90" windowWidth="23895" windowHeight="14535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Release_Plan" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Tên công việc</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Hoàn thành</t>
-  </si>
-  <si>
-    <t>Đã lên kế hoạch</t>
   </si>
   <si>
     <t>Đang trong tiến trình</t>
@@ -422,12 +419,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,6 +434,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,14 +763,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:32" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -835,7 +832,7 @@
         <v>42705.708333333336</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="12"/>
     </row>
@@ -954,7 +951,7 @@
         <v>36</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1229,7 +1226,7 @@
         <v>42705.708333333336</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="5"/>
     </row>
@@ -1247,9 +1244,11 @@
         <v>42702.708333333336</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F24" s="13">
+        <v>42702.708333333336</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1265,9 +1264,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F25" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -1283,9 +1284,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F26" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1301,9 +1304,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F27" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -1319,9 +1324,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F28" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -1337,9 +1344,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F29" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -1355,9 +1364,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F30" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1373,9 +1384,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F31" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -1391,9 +1404,11 @@
         <v>42697.708333333336</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F32" s="13">
+        <v>42697.708333333336</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -1409,9 +1424,11 @@
         <v>42702.708333333336</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F33" s="13">
+        <v>42702.708333333336</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -1427,9 +1444,11 @@
         <v>42702.708333333336</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F34" s="13">
+        <v>42702.708333333336</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -1445,9 +1464,11 @@
         <v>42702.708333333336</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F35" s="13">
+        <v>42702.708333333336</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -1463,9 +1484,11 @@
         <v>42705.708333333336</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="F36" s="13">
+        <v>42705.708333333336</v>
+      </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
@@ -1801,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1815,64 +1838,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>42654</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
-        <v>42654</v>
-      </c>
-      <c r="B2" s="22">
+      <c r="D2" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>42686</v>
+      </c>
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
-        <v>42686</v>
-      </c>
-      <c r="B3" s="22">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>